<commit_message>
fixed tables and reply
</commit_message>
<xml_diff>
--- a/Tables/Table_S6.xlsx
+++ b/Tables/Table_S6.xlsx
@@ -415,14 +415,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>690.1</t>
+          <t>689.4</t>
         </is>
       </c>
       <c r="F2">
-        <v>633.9</v>
+        <v>634.6</v>
       </c>
       <c r="G2">
-        <v>742.5</v>
+        <v>743.1</v>
       </c>
     </row>
     <row r="3">
@@ -446,14 +446,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>43.3</t>
+          <t>44.3</t>
         </is>
       </c>
       <c r="F3">
-        <v>-26.1</v>
+        <v>-24.4</v>
       </c>
       <c r="G3">
-        <v>115.8</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
@@ -477,14 +477,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-28.4</t>
+          <t>-27.4</t>
         </is>
       </c>
       <c r="F4">
-        <v>-97.09999999999999</v>
+        <v>-92.90000000000001</v>
       </c>
       <c r="G4">
-        <v>41.6</v>
+        <v>44.2</v>
       </c>
     </row>
     <row r="5">
@@ -508,14 +508,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-16.4</t>
+          <t>-19.1</t>
         </is>
       </c>
       <c r="F5">
-        <v>-120.9</v>
+        <v>-118.7</v>
       </c>
       <c r="G5">
-        <v>81.8</v>
+        <v>81.40000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -609,14 +609,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>613.3</t>
+          <t>596.5</t>
         </is>
       </c>
       <c r="F9">
-        <v>535.7</v>
+        <v>504.3</v>
       </c>
       <c r="G9">
-        <v>688.2</v>
+        <v>686.6</v>
       </c>
     </row>
     <row r="10">
@@ -640,14 +640,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>235.5</t>
+          <t>250.1</t>
         </is>
       </c>
       <c r="F10">
-        <v>92.40000000000001</v>
+        <v>101</v>
       </c>
       <c r="G10">
-        <v>382.3</v>
+        <v>406.2</v>
       </c>
     </row>
     <row r="11">
@@ -671,14 +671,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>63.5</t>
+          <t>85</t>
         </is>
       </c>
       <c r="F11">
-        <v>-33.9</v>
+        <v>-44</v>
       </c>
       <c r="G11">
-        <v>164.2</v>
+        <v>215.9</v>
       </c>
     </row>
     <row r="12">
@@ -702,14 +702,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-149.2</t>
+          <t>-161.4</t>
         </is>
       </c>
       <c r="F12">
-        <v>-341.2</v>
+        <v>-369.5</v>
       </c>
       <c r="G12">
-        <v>36.4</v>
+        <v>43.6</v>
       </c>
     </row>
     <row r="13">
@@ -733,7 +733,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>19%</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>4%</t>
         </is>
       </c>
     </row>
@@ -778,7 +778,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>77%</t>
         </is>
       </c>
     </row>
@@ -803,14 +803,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>703</t>
+          <t>702.6</t>
         </is>
       </c>
       <c r="F16">
-        <v>648.1</v>
+        <v>649.3</v>
       </c>
       <c r="G16">
-        <v>756.9</v>
+        <v>758.2</v>
       </c>
     </row>
     <row r="17">
@@ -834,14 +834,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>-20.2</t>
+          <t>-19.7</t>
         </is>
       </c>
       <c r="F17">
-        <v>-80</v>
+        <v>-80.3</v>
       </c>
       <c r="G17">
-        <v>41</v>
+        <v>37.9</v>
       </c>
     </row>
     <row r="18">
@@ -865,14 +865,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>-13</t>
+          <t>-12.5</t>
         </is>
       </c>
       <c r="F18">
-        <v>-56.2</v>
+        <v>-54.8</v>
       </c>
       <c r="G18">
-        <v>29.8</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="19">
@@ -896,14 +896,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>27.7</t>
         </is>
       </c>
       <c r="F19">
         <v>-11.5</v>
       </c>
       <c r="G19">
-        <v>66.8</v>
+        <v>66.59999999999999</v>
       </c>
     </row>
     <row r="20">
@@ -927,14 +927,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>18.5</t>
+          <t>17.8</t>
         </is>
       </c>
       <c r="F20">
-        <v>-17.7</v>
+        <v>-19.5</v>
       </c>
       <c r="G20">
-        <v>55.2</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="21">
@@ -958,14 +958,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>42.2</t>
+          <t>42.9</t>
         </is>
       </c>
       <c r="F21">
-        <v>-11.5</v>
+        <v>-11.8</v>
       </c>
       <c r="G21">
-        <v>97.40000000000001</v>
+        <v>96.2</v>
       </c>
     </row>
     <row r="22">
@@ -989,14 +989,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>-2.8</t>
+          <t>-2.6</t>
         </is>
       </c>
       <c r="F22">
-        <v>-59.2</v>
+        <v>-62</v>
       </c>
       <c r="G22">
-        <v>56.7</v>
+        <v>56.9</v>
       </c>
     </row>
     <row r="23">
@@ -1020,14 +1020,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-0.6</t>
+          <t>-1.2</t>
         </is>
       </c>
       <c r="F23">
-        <v>-56.7</v>
+        <v>-55.7</v>
       </c>
       <c r="G23">
-        <v>54.5</v>
+        <v>54.4</v>
       </c>
     </row>
     <row r="24">
@@ -1051,14 +1051,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>31.7</t>
+          <t>33.7</t>
         </is>
       </c>
       <c r="F24">
-        <v>-22.5</v>
+        <v>-22.6</v>
       </c>
       <c r="G24">
-        <v>88.2</v>
+        <v>89.3</v>
       </c>
     </row>
     <row r="25">
@@ -1082,14 +1082,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-77.4</t>
+          <t>-78.6</t>
         </is>
       </c>
       <c r="F25">
-        <v>-160.5</v>
+        <v>-160.4</v>
       </c>
       <c r="G25">
-        <v>5.7</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="26">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>31%</t>
         </is>
       </c>
     </row>

</xml_diff>